<commit_message>
parameterized and ran scenarios for georgia
</commit_message>
<xml_diff>
--- a/diagram_input1.xlsx
+++ b/diagram_input1.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/HCVST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A48F479-E7F4-7A44-A194-ABAD5E631B4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E20193-5A3F-E044-BFA3-283FA505B931}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20480" yWindow="460" windowWidth="20480" windowHeight="22580" xr2:uid="{EA8EDD62-BABB-3F48-AC2F-E4EAD4FEC55C}"/>
+    <workbookView xWindow="20480" yWindow="460" windowWidth="20480" windowHeight="22580" activeTab="1" xr2:uid="{EA8EDD62-BABB-3F48-AC2F-E4EAD4FEC55C}"/>
   </bookViews>
   <sheets>
     <sheet name="Peer-led" sheetId="1" r:id="rId1"/>
     <sheet name="Self-report" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Self-report'!$A$1:$I$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Self-report'!$A$1:$J$69</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="154">
   <si>
     <t>HCV status unknown 1</t>
   </si>
@@ -464,6 +464,42 @@
   </si>
   <si>
     <t>Don't go to health center 72</t>
+  </si>
+  <si>
+    <t>SumGroup</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>ConfirmedAbPos</t>
+  </si>
+  <si>
+    <t>LinkToCare</t>
+  </si>
+  <si>
+    <t>Cured</t>
+  </si>
+  <si>
+    <t>Placeholder</t>
+  </si>
+  <si>
+    <t>SelfTested</t>
+  </si>
+  <si>
+    <t>StandardTested</t>
+  </si>
+  <si>
+    <t>NotConfirmedAbPos</t>
+  </si>
+  <si>
+    <t>DoubleTested</t>
+  </si>
+  <si>
+    <t>UnclearSelfTest</t>
+  </si>
+  <si>
+    <t>NeverTested</t>
   </si>
 </sst>
 </file>
@@ -817,7 +853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726CD0F4-DBF2-814A-A01B-B994F5419C80}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
@@ -2101,19 +2137,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8606919A-616A-2044-AFFD-767D35B1BDB5}">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="2" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -2121,1177 +2157,1384 @@
         <v>130</v>
       </c>
       <c r="C1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" t="s">
         <v>72</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>73</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>74</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>75</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>76</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>78</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>80</v>
       </c>
       <c r="B2" t="s">
         <v>135</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>143</v>
       </c>
       <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>17</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>18</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>136</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>3</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>15</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>137</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>4</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>14</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>138</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>5</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>13</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>139</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6">
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>6</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>12</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>139</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7">
         <v>6</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>7</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>11</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>140</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8">
         <v>7</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>8</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>9</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>10</v>
       </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>131</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9">
         <v>8</v>
       </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>134</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10">
         <v>9</v>
       </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>132</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11">
         <v>10</v>
       </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>132</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12">
         <v>11</v>
       </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>132</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13">
         <v>12</v>
       </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>133</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14">
         <v>13</v>
       </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>132</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15">
         <v>14</v>
       </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>136</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>133</v>
+      </c>
+      <c r="D16">
         <v>15</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>16</v>
       </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>133</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17">
         <v>16</v>
       </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>135</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18">
         <v>17</v>
       </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>135</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19">
         <v>18</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>19</v>
       </c>
-      <c r="E19">
-        <v>20</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>135</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20">
         <v>19</v>
       </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>81</v>
       </c>
       <c r="B21" t="s">
         <v>136</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21">
         <v>20</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>21</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>33</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>50</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>52</v>
       </c>
       <c r="I21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>82</v>
       </c>
       <c r="B22" t="s">
         <v>137</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>144</v>
+      </c>
+      <c r="D22">
         <v>21</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>22</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>23</v>
       </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>83</v>
       </c>
       <c r="B23" t="s">
         <v>132</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>132</v>
+      </c>
+      <c r="D23">
         <v>22</v>
       </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>84</v>
       </c>
       <c r="B24" t="s">
         <v>138</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>138</v>
+      </c>
+      <c r="D24">
         <v>23</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>24</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>32</v>
       </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>85</v>
       </c>
       <c r="B25" t="s">
         <v>139</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>139</v>
+      </c>
+      <c r="D25">
         <v>24</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>25</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>31</v>
       </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>86</v>
       </c>
       <c r="B26" t="s">
         <v>139</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>145</v>
+      </c>
+      <c r="D26">
         <v>25</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>26</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>30</v>
       </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>87</v>
       </c>
       <c r="B27" t="s">
         <v>140</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>140</v>
+      </c>
+      <c r="D27">
         <v>26</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>27</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>28</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>29</v>
       </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>88</v>
       </c>
       <c r="B28" t="s">
         <v>131</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>146</v>
+      </c>
+      <c r="D28">
         <v>27</v>
       </c>
-      <c r="I28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>89</v>
       </c>
       <c r="B29" t="s">
         <v>134</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29">
         <v>28</v>
       </c>
-      <c r="I29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>90</v>
       </c>
       <c r="B30" t="s">
         <v>132</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>132</v>
+      </c>
+      <c r="D30">
         <v>29</v>
       </c>
-      <c r="I30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>91</v>
       </c>
       <c r="B31" t="s">
         <v>132</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>132</v>
+      </c>
+      <c r="D31">
         <v>30</v>
       </c>
-      <c r="I31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>92</v>
       </c>
       <c r="B32" t="s">
         <v>132</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>132</v>
+      </c>
+      <c r="D32">
         <v>31</v>
       </c>
-      <c r="I32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>93</v>
       </c>
       <c r="B33" t="s">
         <v>133</v>
       </c>
-      <c r="C33">
+      <c r="C33" t="s">
+        <v>133</v>
+      </c>
+      <c r="D33">
         <v>32</v>
       </c>
-      <c r="I33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>94</v>
       </c>
       <c r="B34" t="s">
         <v>136</v>
       </c>
-      <c r="C34">
+      <c r="C34" t="s">
+        <v>150</v>
+      </c>
+      <c r="D34">
         <v>33</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>34</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>35</v>
       </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>95</v>
       </c>
       <c r="B35" t="s">
         <v>132</v>
       </c>
-      <c r="C35">
+      <c r="C35" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35">
         <v>34</v>
       </c>
-      <c r="I35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>96</v>
       </c>
       <c r="B36" t="s">
         <v>136</v>
       </c>
-      <c r="C36">
+      <c r="C36" t="s">
+        <v>151</v>
+      </c>
+      <c r="D36">
         <v>35</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>36</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>48</v>
       </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>97</v>
       </c>
       <c r="B37" t="s">
         <v>136</v>
       </c>
-      <c r="C37">
+      <c r="C37" t="s">
+        <v>144</v>
+      </c>
+      <c r="D37">
         <v>36</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>37</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>47</v>
       </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>98</v>
       </c>
       <c r="B38" t="s">
         <v>138</v>
       </c>
-      <c r="C38">
+      <c r="C38" t="s">
+        <v>138</v>
+      </c>
+      <c r="D38">
         <v>37</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>38</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>46</v>
       </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>99</v>
       </c>
       <c r="B39" t="s">
         <v>139</v>
       </c>
-      <c r="C39">
+      <c r="C39" t="s">
+        <v>139</v>
+      </c>
+      <c r="D39">
         <v>38</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>39</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>45</v>
       </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>100</v>
       </c>
       <c r="B40" t="s">
         <v>139</v>
       </c>
-      <c r="C40">
+      <c r="C40" t="s">
+        <v>145</v>
+      </c>
+      <c r="D40">
         <v>39</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>40</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>44</v>
       </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>101</v>
       </c>
       <c r="B41" t="s">
         <v>140</v>
       </c>
-      <c r="C41">
+      <c r="C41" t="s">
+        <v>140</v>
+      </c>
+      <c r="D41">
         <v>40</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>41</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>42</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>43</v>
       </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>102</v>
       </c>
       <c r="B42" t="s">
         <v>131</v>
       </c>
-      <c r="C42">
+      <c r="C42" t="s">
+        <v>146</v>
+      </c>
+      <c r="D42">
         <v>41</v>
       </c>
-      <c r="I42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>103</v>
       </c>
       <c r="B43" t="s">
         <v>134</v>
       </c>
-      <c r="C43">
+      <c r="C43" t="s">
+        <v>134</v>
+      </c>
+      <c r="D43">
         <v>42</v>
       </c>
-      <c r="I43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>104</v>
       </c>
       <c r="B44" t="s">
         <v>132</v>
       </c>
-      <c r="C44">
+      <c r="C44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D44">
         <v>43</v>
       </c>
-      <c r="I44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>105</v>
       </c>
       <c r="B45" t="s">
         <v>132</v>
       </c>
-      <c r="C45">
+      <c r="C45" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45">
         <v>44</v>
       </c>
-      <c r="I45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>106</v>
       </c>
       <c r="B46" t="s">
         <v>132</v>
       </c>
-      <c r="C46">
+      <c r="C46" t="s">
+        <v>132</v>
+      </c>
+      <c r="D46">
         <v>45</v>
       </c>
-      <c r="I46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>107</v>
       </c>
       <c r="B47" t="s">
         <v>133</v>
       </c>
-      <c r="C47">
+      <c r="C47" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47">
         <v>46</v>
       </c>
-      <c r="I47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>108</v>
       </c>
       <c r="B48" t="s">
         <v>132</v>
       </c>
-      <c r="C48">
+      <c r="C48" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48">
         <v>47</v>
       </c>
-      <c r="I48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>109</v>
       </c>
       <c r="B49" t="s">
         <v>136</v>
       </c>
-      <c r="C49">
+      <c r="C49" t="s">
+        <v>133</v>
+      </c>
+      <c r="D49">
         <v>48</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <v>49</v>
       </c>
-      <c r="I49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>110</v>
       </c>
       <c r="B50" t="s">
         <v>133</v>
       </c>
-      <c r="C50">
+      <c r="C50" t="s">
+        <v>147</v>
+      </c>
+      <c r="D50">
         <v>49</v>
       </c>
-      <c r="I50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>111</v>
       </c>
       <c r="B51" t="s">
         <v>136</v>
       </c>
-      <c r="C51">
+      <c r="C51" t="s">
+        <v>133</v>
+      </c>
+      <c r="D51">
         <v>50</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <v>51</v>
       </c>
-      <c r="I51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>112</v>
       </c>
       <c r="B52" t="s">
         <v>133</v>
       </c>
-      <c r="C52">
+      <c r="C52" t="s">
+        <v>147</v>
+      </c>
+      <c r="D52">
         <v>51</v>
       </c>
-      <c r="I52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>113</v>
       </c>
       <c r="B53" t="s">
         <v>136</v>
       </c>
-      <c r="C53">
+      <c r="C53" t="s">
+        <v>152</v>
+      </c>
+      <c r="D53">
         <v>52</v>
       </c>
-      <c r="D53">
+      <c r="E53">
         <v>53</v>
       </c>
-      <c r="E53">
+      <c r="F53">
         <v>54</v>
       </c>
-      <c r="I53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>114</v>
       </c>
       <c r="B54" t="s">
         <v>132</v>
       </c>
-      <c r="C54">
+      <c r="C54" t="s">
+        <v>132</v>
+      </c>
+      <c r="D54">
         <v>53</v>
       </c>
-      <c r="I54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>115</v>
       </c>
       <c r="B55" t="s">
         <v>136</v>
       </c>
-      <c r="C55">
+      <c r="C55" t="s">
+        <v>151</v>
+      </c>
+      <c r="D55">
         <v>54</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <v>55</v>
       </c>
-      <c r="E55">
+      <c r="F55">
         <v>67</v>
       </c>
-      <c r="I55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>116</v>
       </c>
       <c r="B56" t="s">
         <v>137</v>
       </c>
-      <c r="C56">
+      <c r="C56" t="s">
+        <v>144</v>
+      </c>
+      <c r="D56">
         <v>55</v>
       </c>
-      <c r="D56">
+      <c r="E56">
         <v>56</v>
       </c>
-      <c r="E56">
+      <c r="F56">
         <v>66</v>
       </c>
-      <c r="I56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>117</v>
       </c>
       <c r="B57" t="s">
         <v>138</v>
       </c>
-      <c r="C57">
+      <c r="C57" t="s">
+        <v>138</v>
+      </c>
+      <c r="D57">
         <v>56</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <v>57</v>
       </c>
-      <c r="E57">
+      <c r="F57">
         <v>65</v>
       </c>
-      <c r="I57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>118</v>
       </c>
       <c r="B58" t="s">
         <v>139</v>
       </c>
-      <c r="C58">
+      <c r="C58" t="s">
+        <v>139</v>
+      </c>
+      <c r="D58">
         <v>57</v>
       </c>
-      <c r="D58">
+      <c r="E58">
         <v>58</v>
       </c>
-      <c r="E58">
+      <c r="F58">
         <v>64</v>
       </c>
-      <c r="I58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>119</v>
       </c>
       <c r="B59" t="s">
         <v>139</v>
       </c>
-      <c r="C59">
+      <c r="C59" t="s">
+        <v>145</v>
+      </c>
+      <c r="D59">
         <v>58</v>
       </c>
-      <c r="D59">
+      <c r="E59">
         <v>59</v>
       </c>
-      <c r="E59">
+      <c r="F59">
         <v>63</v>
       </c>
-      <c r="I59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>120</v>
       </c>
       <c r="B60" t="s">
         <v>140</v>
       </c>
-      <c r="C60">
+      <c r="C60" t="s">
+        <v>140</v>
+      </c>
+      <c r="D60">
         <v>59</v>
       </c>
-      <c r="D60">
+      <c r="E60">
         <v>60</v>
       </c>
-      <c r="E60">
+      <c r="F60">
         <v>61</v>
       </c>
-      <c r="F60">
+      <c r="G60">
         <v>62</v>
       </c>
-      <c r="I60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>121</v>
       </c>
       <c r="B61" t="s">
         <v>131</v>
       </c>
-      <c r="C61">
+      <c r="C61" t="s">
+        <v>146</v>
+      </c>
+      <c r="D61">
         <v>60</v>
       </c>
-      <c r="I61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>122</v>
       </c>
       <c r="B62" t="s">
         <v>134</v>
       </c>
-      <c r="C62">
+      <c r="C62" t="s">
+        <v>134</v>
+      </c>
+      <c r="D62">
         <v>61</v>
       </c>
-      <c r="I62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>123</v>
       </c>
       <c r="B63" t="s">
         <v>132</v>
       </c>
-      <c r="C63">
+      <c r="C63" t="s">
+        <v>132</v>
+      </c>
+      <c r="D63">
         <v>62</v>
       </c>
-      <c r="I63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>124</v>
       </c>
       <c r="B64" t="s">
         <v>132</v>
       </c>
-      <c r="C64">
+      <c r="C64" t="s">
+        <v>132</v>
+      </c>
+      <c r="D64">
         <v>63</v>
       </c>
-      <c r="I64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>125</v>
       </c>
       <c r="B65" t="s">
         <v>132</v>
       </c>
-      <c r="C65">
+      <c r="C65" t="s">
+        <v>132</v>
+      </c>
+      <c r="D65">
         <v>64</v>
       </c>
-      <c r="I65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>126</v>
       </c>
       <c r="B66" t="s">
         <v>133</v>
       </c>
-      <c r="C66">
+      <c r="C66" t="s">
+        <v>133</v>
+      </c>
+      <c r="D66">
         <v>65</v>
       </c>
-      <c r="I66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>127</v>
       </c>
       <c r="B67" t="s">
         <v>132</v>
       </c>
-      <c r="C67">
+      <c r="C67" t="s">
+        <v>132</v>
+      </c>
+      <c r="D67">
         <v>66</v>
       </c>
-      <c r="I67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>128</v>
       </c>
       <c r="B68" t="s">
         <v>136</v>
       </c>
-      <c r="C68">
+      <c r="C68" t="s">
+        <v>133</v>
+      </c>
+      <c r="D68">
         <v>67</v>
       </c>
-      <c r="D68">
+      <c r="E68">
         <v>68</v>
       </c>
-      <c r="I68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>129</v>
       </c>
       <c r="B69" t="s">
         <v>133</v>
       </c>
-      <c r="C69">
+      <c r="C69" t="s">
+        <v>133</v>
+      </c>
+      <c r="D69">
         <v>68</v>
       </c>
-      <c r="I69">
+      <c r="J69">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ran same scenarios for each setting with different parameter inputs
</commit_message>
<xml_diff>
--- a/diagram_input1.xlsx
+++ b/diagram_input1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/HCVST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E20193-5A3F-E044-BFA3-283FA505B931}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF037024-2E64-C84C-82FC-1687645848F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20480" yWindow="460" windowWidth="20480" windowHeight="22580" activeTab="1" xr2:uid="{EA8EDD62-BABB-3F48-AC2F-E4EAD4FEC55C}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Self-report" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Self-report'!$A$1:$J$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Self-report'!$A$1:$J$68</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="154">
   <si>
     <t>HCV status unknown 1</t>
   </si>
@@ -283,9 +283,6 @@
     <t>HCV Status unknown 1</t>
   </si>
   <si>
-    <t>Result brought to health center 20</t>
-  </si>
-  <si>
     <t>Positive Ab  trusted 21</t>
   </si>
   <si>
@@ -500,6 +497,9 @@
   </si>
   <si>
     <t>NeverTested</t>
+  </si>
+  <si>
+    <t>Self-testing 20</t>
   </si>
 </sst>
 </file>
@@ -868,7 +868,7 @@
         <v>71</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C1" t="s">
         <v>72</v>
@@ -897,7 +897,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -920,7 +920,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -940,7 +940,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -960,7 +960,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -980,7 +980,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -1000,7 +1000,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -1020,7 +1020,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1043,7 +1043,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -1057,7 +1057,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -1071,7 +1071,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -1085,7 +1085,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C12">
         <v>11</v>
@@ -1099,7 +1099,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -1113,7 +1113,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C14">
         <v>13</v>
@@ -1127,7 +1127,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -1141,7 +1141,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -1158,7 +1158,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C17">
         <v>16</v>
@@ -1172,7 +1172,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C18">
         <v>17</v>
@@ -1186,7 +1186,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C19">
         <v>18</v>
@@ -1215,7 +1215,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C20">
         <v>19</v>
@@ -1229,7 +1229,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -1249,7 +1249,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C22">
         <v>21</v>
@@ -1269,7 +1269,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -1289,7 +1289,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C24">
         <v>23</v>
@@ -1309,7 +1309,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C25">
         <v>24</v>
@@ -1329,7 +1329,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C26">
         <v>25</v>
@@ -1352,7 +1352,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C27">
         <v>26</v>
@@ -1366,7 +1366,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C28">
         <v>27</v>
@@ -1380,7 +1380,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C29">
         <v>28</v>
@@ -1394,7 +1394,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C30">
         <v>29</v>
@@ -1408,7 +1408,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C31">
         <v>30</v>
@@ -1422,7 +1422,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C32">
         <v>31</v>
@@ -1436,7 +1436,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C33">
         <v>32</v>
@@ -1450,7 +1450,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C34">
         <v>33</v>
@@ -1470,7 +1470,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C35">
         <v>34</v>
@@ -1490,7 +1490,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C36">
         <v>35</v>
@@ -1504,7 +1504,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C37">
         <v>36</v>
@@ -1524,7 +1524,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C38">
         <v>37</v>
@@ -1544,7 +1544,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C39">
         <v>38</v>
@@ -1564,7 +1564,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C40">
         <v>39</v>
@@ -1584,7 +1584,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C41">
         <v>40</v>
@@ -1604,7 +1604,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C42">
         <v>41</v>
@@ -1627,7 +1627,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C43">
         <v>42</v>
@@ -1641,7 +1641,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C44">
         <v>43</v>
@@ -1655,7 +1655,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C45">
         <v>44</v>
@@ -1669,7 +1669,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C46">
         <v>45</v>
@@ -1683,7 +1683,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C47">
         <v>46</v>
@@ -1697,7 +1697,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C48">
         <v>47</v>
@@ -1711,7 +1711,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C49">
         <v>48</v>
@@ -1725,7 +1725,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C50">
         <v>49</v>
@@ -1742,7 +1742,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C51">
         <v>50</v>
@@ -1756,7 +1756,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C52">
         <v>51</v>
@@ -1770,7 +1770,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C53">
         <v>52</v>
@@ -1787,7 +1787,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C54">
         <v>53</v>
@@ -1801,7 +1801,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C55">
         <v>54</v>
@@ -1821,7 +1821,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C56">
         <v>55</v>
@@ -1841,7 +1841,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C57">
         <v>56</v>
@@ -1855,7 +1855,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C58">
         <v>57</v>
@@ -1875,7 +1875,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C59">
         <v>58</v>
@@ -1895,7 +1895,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C60">
         <v>59</v>
@@ -1915,7 +1915,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C61">
         <v>60</v>
@@ -1935,7 +1935,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C62">
         <v>61</v>
@@ -1955,7 +1955,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C63">
         <v>62</v>
@@ -1978,7 +1978,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C64">
         <v>63</v>
@@ -1992,7 +1992,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C65">
         <v>64</v>
@@ -2006,7 +2006,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C66">
         <v>65</v>
@@ -2020,7 +2020,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C67">
         <v>66</v>
@@ -2034,7 +2034,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C68">
         <v>67</v>
@@ -2048,7 +2048,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C69">
         <v>68</v>
@@ -2062,7 +2062,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C70">
         <v>69</v>
@@ -2076,7 +2076,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C71">
         <v>70</v>
@@ -2093,7 +2093,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C72">
         <v>71</v>
@@ -2104,10 +2104,10 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B73" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C73">
         <v>72</v>
@@ -2121,7 +2121,7 @@
         <v>79</v>
       </c>
       <c r="B74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C74">
         <v>73</v>
@@ -2137,10 +2137,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8606919A-616A-2044-AFFD-767D35B1BDB5}">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2154,10 +2154,10 @@
         <v>71</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D1" t="s">
         <v>72</v>
@@ -2186,10 +2186,10 @@
         <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2201,7 +2201,7 @@
         <v>17</v>
       </c>
       <c r="G2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -2212,10 +2212,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -2235,10 +2235,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -2258,10 +2258,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -2281,10 +2281,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -2304,10 +2304,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -2327,10 +2327,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -2353,10 +2353,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -2370,10 +2370,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -2387,10 +2387,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -2404,10 +2404,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D12">
         <v>11</v>
@@ -2421,10 +2421,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D13">
         <v>12</v>
@@ -2438,10 +2438,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D14">
         <v>13</v>
@@ -2455,10 +2455,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D15">
         <v>14</v>
@@ -2472,10 +2472,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D16">
         <v>15</v>
@@ -2492,10 +2492,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D17">
         <v>16</v>
@@ -2509,10 +2509,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D18">
         <v>17</v>
@@ -2523,39 +2523,51 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="D19">
-        <v>18</v>
-      </c>
-      <c r="E19">
         <v>19</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="B20" t="s">
         <v>135</v>
       </c>
       <c r="C20" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="E20">
+        <v>21</v>
+      </c>
+      <c r="F20">
+        <v>33</v>
+      </c>
+      <c r="G20">
+        <v>50</v>
+      </c>
+      <c r="H20">
+        <v>52</v>
+      </c>
+      <c r="I20">
         <v>19</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -2566,25 +2578,16 @@
         <v>136</v>
       </c>
       <c r="C21" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E21">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F21">
-        <v>33</v>
-      </c>
-      <c r="G21">
-        <v>50</v>
-      </c>
-      <c r="H21">
-        <v>52</v>
-      </c>
-      <c r="I21">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -2595,22 +2598,16 @@
         <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C22" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="D22">
-        <v>21</v>
-      </c>
-      <c r="E22">
         <v>22</v>
       </c>
-      <c r="F22">
-        <v>23</v>
-      </c>
       <c r="J22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -2618,16 +2615,22 @@
         <v>83</v>
       </c>
       <c r="B23" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C23" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D23">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="E23">
+        <v>24</v>
+      </c>
+      <c r="F23">
+        <v>32</v>
       </c>
       <c r="J23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -2641,13 +2644,13 @@
         <v>138</v>
       </c>
       <c r="D24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E24">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F24">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -2658,19 +2661,19 @@
         <v>85</v>
       </c>
       <c r="B25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C25" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D25">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E25">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F25">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J25">
         <v>0</v>
@@ -2684,16 +2687,19 @@
         <v>139</v>
       </c>
       <c r="C26" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D26">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E26">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F26">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="G26">
+        <v>29</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -2704,25 +2710,16 @@
         <v>87</v>
       </c>
       <c r="B27" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C27" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D27">
-        <v>26</v>
-      </c>
-      <c r="E27">
         <v>27</v>
       </c>
-      <c r="F27">
-        <v>28</v>
-      </c>
-      <c r="G27">
-        <v>29</v>
-      </c>
       <c r="J27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -2730,13 +2727,13 @@
         <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C28" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="D28">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -2747,13 +2744,13 @@
         <v>89</v>
       </c>
       <c r="B29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D29">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J29">
         <v>1</v>
@@ -2764,13 +2761,13 @@
         <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D30">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -2781,13 +2778,13 @@
         <v>91</v>
       </c>
       <c r="B31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D31">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J31">
         <v>1</v>
@@ -2804,7 +2801,7 @@
         <v>132</v>
       </c>
       <c r="D32">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J32">
         <v>1</v>
@@ -2815,16 +2812,22 @@
         <v>93</v>
       </c>
       <c r="B33" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C33" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="D33">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="E33">
+        <v>34</v>
+      </c>
+      <c r="F33">
+        <v>35</v>
       </c>
       <c r="J33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -2832,22 +2835,16 @@
         <v>94</v>
       </c>
       <c r="B34" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C34" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="D34">
-        <v>33</v>
-      </c>
-      <c r="E34">
         <v>34</v>
       </c>
-      <c r="F34">
-        <v>35</v>
-      </c>
       <c r="J34">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -2855,16 +2852,22 @@
         <v>95</v>
       </c>
       <c r="B35" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C35" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="D35">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="E35">
+        <v>36</v>
+      </c>
+      <c r="F35">
+        <v>48</v>
       </c>
       <c r="J35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -2872,19 +2875,19 @@
         <v>96</v>
       </c>
       <c r="B36" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C36" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D36">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E36">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F36">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J36">
         <v>0</v>
@@ -2895,19 +2898,19 @@
         <v>97</v>
       </c>
       <c r="B37" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C37" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D37">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E37">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F37">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J37">
         <v>0</v>
@@ -2924,13 +2927,13 @@
         <v>138</v>
       </c>
       <c r="D38">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E38">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F38">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -2941,19 +2944,19 @@
         <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C39" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D39">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E39">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F39">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J39">
         <v>0</v>
@@ -2967,16 +2970,19 @@
         <v>139</v>
       </c>
       <c r="C40" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D40">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E40">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F40">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="G40">
+        <v>43</v>
       </c>
       <c r="J40">
         <v>0</v>
@@ -2987,25 +2993,16 @@
         <v>101</v>
       </c>
       <c r="B41" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C41" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D41">
-        <v>40</v>
-      </c>
-      <c r="E41">
         <v>41</v>
       </c>
-      <c r="F41">
-        <v>42</v>
-      </c>
-      <c r="G41">
-        <v>43</v>
-      </c>
       <c r="J41">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -3013,13 +3010,13 @@
         <v>102</v>
       </c>
       <c r="B42" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C42" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="D42">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J42">
         <v>1</v>
@@ -3030,13 +3027,13 @@
         <v>103</v>
       </c>
       <c r="B43" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C43" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D43">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J43">
         <v>1</v>
@@ -3047,13 +3044,13 @@
         <v>104</v>
       </c>
       <c r="B44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D44">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J44">
         <v>1</v>
@@ -3064,13 +3061,13 @@
         <v>105</v>
       </c>
       <c r="B45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D45">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J45">
         <v>1</v>
@@ -3087,7 +3084,7 @@
         <v>132</v>
       </c>
       <c r="D46">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J46">
         <v>1</v>
@@ -3098,13 +3095,13 @@
         <v>107</v>
       </c>
       <c r="B47" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C47" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D47">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J47">
         <v>1</v>
@@ -3115,16 +3112,19 @@
         <v>108</v>
       </c>
       <c r="B48" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C48" t="s">
         <v>132</v>
       </c>
       <c r="D48">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="E48">
+        <v>49</v>
       </c>
       <c r="J48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
@@ -3132,19 +3132,16 @@
         <v>109</v>
       </c>
       <c r="B49" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C49" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="D49">
-        <v>48</v>
-      </c>
-      <c r="E49">
         <v>49</v>
       </c>
       <c r="J49">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -3152,16 +3149,19 @@
         <v>110</v>
       </c>
       <c r="B50" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C50" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="D50">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="E50">
+        <v>51</v>
       </c>
       <c r="J50">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -3169,19 +3169,16 @@
         <v>111</v>
       </c>
       <c r="B51" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C51" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="D51">
-        <v>50</v>
-      </c>
-      <c r="E51">
         <v>51</v>
       </c>
       <c r="J51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
@@ -3189,16 +3186,22 @@
         <v>112</v>
       </c>
       <c r="B52" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C52" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D52">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="E52">
+        <v>53</v>
+      </c>
+      <c r="F52">
+        <v>54</v>
       </c>
       <c r="J52">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
@@ -3206,22 +3209,16 @@
         <v>113</v>
       </c>
       <c r="B53" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C53" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="D53">
-        <v>52</v>
-      </c>
-      <c r="E53">
         <v>53</v>
       </c>
-      <c r="F53">
-        <v>54</v>
-      </c>
       <c r="J53">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
@@ -3229,16 +3226,22 @@
         <v>114</v>
       </c>
       <c r="B54" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C54" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="D54">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="E54">
+        <v>55</v>
+      </c>
+      <c r="F54">
+        <v>67</v>
       </c>
       <c r="J54">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -3249,16 +3252,16 @@
         <v>136</v>
       </c>
       <c r="C55" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D55">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E55">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F55">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J55">
         <v>0</v>
@@ -3272,16 +3275,16 @@
         <v>137</v>
       </c>
       <c r="C56" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D56">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E56">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F56">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J56">
         <v>0</v>
@@ -3298,13 +3301,13 @@
         <v>138</v>
       </c>
       <c r="D57">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E57">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F57">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J57">
         <v>0</v>
@@ -3315,19 +3318,19 @@
         <v>118</v>
       </c>
       <c r="B58" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C58" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D58">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E58">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F58">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J58">
         <v>0</v>
@@ -3341,16 +3344,19 @@
         <v>139</v>
       </c>
       <c r="C59" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D59">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E59">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F59">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="G59">
+        <v>62</v>
       </c>
       <c r="J59">
         <v>0</v>
@@ -3361,25 +3367,16 @@
         <v>120</v>
       </c>
       <c r="B60" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C60" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D60">
-        <v>59</v>
-      </c>
-      <c r="E60">
         <v>60</v>
       </c>
-      <c r="F60">
-        <v>61</v>
-      </c>
-      <c r="G60">
-        <v>62</v>
-      </c>
       <c r="J60">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
@@ -3387,13 +3384,13 @@
         <v>121</v>
       </c>
       <c r="B61" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C61" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="D61">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J61">
         <v>1</v>
@@ -3404,13 +3401,13 @@
         <v>122</v>
       </c>
       <c r="B62" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C62" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D62">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J62">
         <v>1</v>
@@ -3421,13 +3418,13 @@
         <v>123</v>
       </c>
       <c r="B63" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C63" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D63">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J63">
         <v>1</v>
@@ -3438,13 +3435,13 @@
         <v>124</v>
       </c>
       <c r="B64" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C64" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D64">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J64">
         <v>1</v>
@@ -3461,7 +3458,7 @@
         <v>132</v>
       </c>
       <c r="D65">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J65">
         <v>1</v>
@@ -3472,13 +3469,13 @@
         <v>126</v>
       </c>
       <c r="B66" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C66" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D66">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J66">
         <v>1</v>
@@ -3489,16 +3486,19 @@
         <v>127</v>
       </c>
       <c r="B67" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C67" t="s">
         <v>132</v>
       </c>
       <c r="D67">
-        <v>66</v>
+        <v>67</v>
+      </c>
+      <c r="E67">
+        <v>68</v>
       </c>
       <c r="J67">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
@@ -3506,35 +3506,15 @@
         <v>128</v>
       </c>
       <c r="B68" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C68" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D68">
-        <v>67</v>
-      </c>
-      <c r="E68">
         <v>68</v>
       </c>
       <c r="J68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>129</v>
-      </c>
-      <c r="B69" t="s">
-        <v>133</v>
-      </c>
-      <c r="C69" t="s">
-        <v>133</v>
-      </c>
-      <c r="D69">
-        <v>68</v>
-      </c>
-      <c r="J69">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
apparently changed some things previously
</commit_message>
<xml_diff>
--- a/diagram_input1.xlsx
+++ b/diagram_input1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/HCVST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF037024-2E64-C84C-82FC-1687645848F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF17042-F1ED-FC4E-BE5C-E47F009FE2AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20480" yWindow="460" windowWidth="20480" windowHeight="22580" activeTab="1" xr2:uid="{EA8EDD62-BABB-3F48-AC2F-E4EAD4FEC55C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="22580" activeTab="1" xr2:uid="{EA8EDD62-BABB-3F48-AC2F-E4EAD4FEC55C}"/>
   </bookViews>
   <sheets>
     <sheet name="Peer-led" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Self-report'!$A$1:$J$68</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2140,7 +2140,7 @@
   <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fixed bug with adding up numbers within cascade
</commit_message>
<xml_diff>
--- a/diagram_input1.xlsx
+++ b/diagram_input1.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/HCVST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF17042-F1ED-FC4E-BE5C-E47F009FE2AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA325823-6F27-3945-8B6E-AD1A3E8BCC3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="22580" activeTab="1" xr2:uid="{EA8EDD62-BABB-3F48-AC2F-E4EAD4FEC55C}"/>
+    <workbookView xWindow="12400" yWindow="920" windowWidth="20480" windowHeight="22580" activeTab="1" xr2:uid="{EA8EDD62-BABB-3F48-AC2F-E4EAD4FEC55C}"/>
   </bookViews>
   <sheets>
     <sheet name="Peer-led" sheetId="1" r:id="rId1"/>
     <sheet name="Self-report" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Self-report'!$A$1:$J$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Self-report'!$A$1:$K$68</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="155">
   <si>
     <t>HCV status unknown 1</t>
   </si>
@@ -500,6 +500,9 @@
   </si>
   <si>
     <t>Self-testing 20</t>
+  </si>
+  <si>
+    <t>SumGroup1</t>
   </si>
 </sst>
 </file>
@@ -853,7 +856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726CD0F4-DBF2-814A-A01B-B994F5419C80}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
@@ -2137,19 +2140,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8606919A-616A-2044-AFFD-767D35B1BDB5}">
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -2160,28 +2164,31 @@
         <v>141</v>
       </c>
       <c r="D1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" t="s">
         <v>72</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>73</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>74</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>75</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>76</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>78</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -2195,19 +2202,22 @@
         <v>1</v>
       </c>
       <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>17</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>20</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2221,16 +2231,19 @@
         <v>2</v>
       </c>
       <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
         <v>3</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>15</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2244,16 +2257,19 @@
         <v>3</v>
       </c>
       <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
         <v>4</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>14</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2267,16 +2283,19 @@
         <v>4</v>
       </c>
       <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
         <v>5</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>13</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2290,16 +2309,19 @@
         <v>5</v>
       </c>
       <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
         <v>6</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>12</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2313,16 +2335,19 @@
         <v>6</v>
       </c>
       <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
         <v>7</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>11</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2336,19 +2361,22 @@
         <v>7</v>
       </c>
       <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
         <v>8</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>9</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>10</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2361,11 +2389,14 @@
       <c r="D9">
         <v>8</v>
       </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2378,11 +2409,14 @@
       <c r="D10">
         <v>9</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2395,11 +2429,14 @@
       <c r="D11">
         <v>10</v>
       </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2412,11 +2449,14 @@
       <c r="D12">
         <v>11</v>
       </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2429,11 +2469,14 @@
       <c r="D13">
         <v>12</v>
       </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2446,11 +2489,14 @@
       <c r="D14">
         <v>13</v>
       </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>13</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2463,11 +2509,14 @@
       <c r="D15">
         <v>14</v>
       </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>14</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2481,13 +2530,16 @@
         <v>15</v>
       </c>
       <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
         <v>16</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2500,11 +2552,14 @@
       <c r="D17">
         <v>16</v>
       </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2517,11 +2572,14 @@
       <c r="D18">
         <v>17</v>
       </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>17</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2534,11 +2592,14 @@
       <c r="D19">
         <v>19</v>
       </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>19</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>153</v>
       </c>
@@ -2552,25 +2613,28 @@
         <v>20</v>
       </c>
       <c r="E20">
+        <v>20</v>
+      </c>
+      <c r="F20">
         <v>21</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>33</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>50</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>52</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>19</v>
       </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -2584,16 +2648,19 @@
         <v>21</v>
       </c>
       <c r="E21">
+        <v>21</v>
+      </c>
+      <c r="F21">
         <v>22</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>23</v>
       </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -2606,11 +2673,14 @@
       <c r="D22">
         <v>22</v>
       </c>
-      <c r="J22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>22</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>83</v>
       </c>
@@ -2624,16 +2694,19 @@
         <v>23</v>
       </c>
       <c r="E23">
+        <v>23</v>
+      </c>
+      <c r="F23">
         <v>24</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>32</v>
       </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -2647,16 +2720,19 @@
         <v>24</v>
       </c>
       <c r="E24">
+        <v>24</v>
+      </c>
+      <c r="F24">
         <v>25</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>31</v>
       </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>85</v>
       </c>
@@ -2670,16 +2746,19 @@
         <v>25</v>
       </c>
       <c r="E25">
+        <v>25</v>
+      </c>
+      <c r="F25">
         <v>26</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>30</v>
       </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>86</v>
       </c>
@@ -2693,19 +2772,22 @@
         <v>26</v>
       </c>
       <c r="E26">
+        <v>26</v>
+      </c>
+      <c r="F26">
         <v>27</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>28</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>29</v>
       </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>87</v>
       </c>
@@ -2718,11 +2800,14 @@
       <c r="D27">
         <v>27</v>
       </c>
-      <c r="J27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>27</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -2735,11 +2820,14 @@
       <c r="D28">
         <v>28</v>
       </c>
-      <c r="J28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>28</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>89</v>
       </c>
@@ -2752,11 +2840,14 @@
       <c r="D29">
         <v>29</v>
       </c>
-      <c r="J29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>29</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>90</v>
       </c>
@@ -2769,11 +2860,14 @@
       <c r="D30">
         <v>30</v>
       </c>
-      <c r="J30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>30</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>91</v>
       </c>
@@ -2786,11 +2880,14 @@
       <c r="D31">
         <v>31</v>
       </c>
-      <c r="J31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>31</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>92</v>
       </c>
@@ -2803,11 +2900,14 @@
       <c r="D32">
         <v>32</v>
       </c>
-      <c r="J32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>32</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>93</v>
       </c>
@@ -2821,16 +2921,19 @@
         <v>33</v>
       </c>
       <c r="E33">
+        <v>33</v>
+      </c>
+      <c r="F33">
         <v>34</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>35</v>
       </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>94</v>
       </c>
@@ -2843,11 +2946,14 @@
       <c r="D34">
         <v>34</v>
       </c>
-      <c r="J34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>34</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>95</v>
       </c>
@@ -2861,16 +2967,19 @@
         <v>35</v>
       </c>
       <c r="E35">
+        <v>35</v>
+      </c>
+      <c r="F35">
         <v>36</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>48</v>
       </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>96</v>
       </c>
@@ -2884,16 +2993,19 @@
         <v>36</v>
       </c>
       <c r="E36">
+        <v>36</v>
+      </c>
+      <c r="F36">
         <v>37</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>47</v>
       </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -2907,16 +3019,19 @@
         <v>37</v>
       </c>
       <c r="E37">
+        <v>37</v>
+      </c>
+      <c r="F37">
         <v>38</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>46</v>
       </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>98</v>
       </c>
@@ -2930,16 +3045,19 @@
         <v>38</v>
       </c>
       <c r="E38">
+        <v>38</v>
+      </c>
+      <c r="F38">
         <v>39</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>45</v>
       </c>
-      <c r="J38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>99</v>
       </c>
@@ -2953,16 +3071,19 @@
         <v>39</v>
       </c>
       <c r="E39">
+        <v>39</v>
+      </c>
+      <c r="F39">
         <v>40</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>44</v>
       </c>
-      <c r="J39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>100</v>
       </c>
@@ -2976,19 +3097,22 @@
         <v>40</v>
       </c>
       <c r="E40">
+        <v>40</v>
+      </c>
+      <c r="F40">
         <v>41</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>42</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>43</v>
       </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>101</v>
       </c>
@@ -3001,11 +3125,14 @@
       <c r="D41">
         <v>41</v>
       </c>
-      <c r="J41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>41</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>102</v>
       </c>
@@ -3018,11 +3145,14 @@
       <c r="D42">
         <v>42</v>
       </c>
-      <c r="J42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>42</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>103</v>
       </c>
@@ -3035,11 +3165,14 @@
       <c r="D43">
         <v>43</v>
       </c>
-      <c r="J43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <v>43</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>104</v>
       </c>
@@ -3052,11 +3185,14 @@
       <c r="D44">
         <v>44</v>
       </c>
-      <c r="J44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <v>44</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>105</v>
       </c>
@@ -3069,11 +3205,14 @@
       <c r="D45">
         <v>45</v>
       </c>
-      <c r="J45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E45">
+        <v>45</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>106</v>
       </c>
@@ -3086,11 +3225,14 @@
       <c r="D46">
         <v>46</v>
       </c>
-      <c r="J46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <v>46</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>107</v>
       </c>
@@ -3103,11 +3245,14 @@
       <c r="D47">
         <v>47</v>
       </c>
-      <c r="J47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E47">
+        <v>47</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>108</v>
       </c>
@@ -3121,13 +3266,16 @@
         <v>48</v>
       </c>
       <c r="E48">
+        <v>48</v>
+      </c>
+      <c r="F48">
         <v>49</v>
       </c>
-      <c r="J48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>109</v>
       </c>
@@ -3140,11 +3288,14 @@
       <c r="D49">
         <v>49</v>
       </c>
-      <c r="J49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <v>49</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>110</v>
       </c>
@@ -3158,13 +3309,16 @@
         <v>50</v>
       </c>
       <c r="E50">
+        <v>50</v>
+      </c>
+      <c r="F50">
         <v>51</v>
       </c>
-      <c r="J50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>111</v>
       </c>
@@ -3177,11 +3331,14 @@
       <c r="D51">
         <v>51</v>
       </c>
-      <c r="J51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E51">
+        <v>51</v>
+      </c>
+      <c r="K51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>112</v>
       </c>
@@ -3195,16 +3352,19 @@
         <v>52</v>
       </c>
       <c r="E52">
+        <v>52</v>
+      </c>
+      <c r="F52">
         <v>53</v>
       </c>
-      <c r="F52">
+      <c r="G52">
         <v>54</v>
       </c>
-      <c r="J52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>113</v>
       </c>
@@ -3217,11 +3377,14 @@
       <c r="D53">
         <v>53</v>
       </c>
-      <c r="J53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E53">
+        <v>53</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>114</v>
       </c>
@@ -3235,16 +3398,19 @@
         <v>54</v>
       </c>
       <c r="E54">
+        <v>54</v>
+      </c>
+      <c r="F54">
         <v>55</v>
       </c>
-      <c r="F54">
+      <c r="G54">
         <v>67</v>
       </c>
-      <c r="J54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>115</v>
       </c>
@@ -3258,16 +3424,19 @@
         <v>55</v>
       </c>
       <c r="E55">
+        <v>55</v>
+      </c>
+      <c r="F55">
         <v>56</v>
       </c>
-      <c r="F55">
+      <c r="G55">
         <v>66</v>
       </c>
-      <c r="J55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>116</v>
       </c>
@@ -3281,16 +3450,19 @@
         <v>56</v>
       </c>
       <c r="E56">
+        <v>56</v>
+      </c>
+      <c r="F56">
         <v>57</v>
       </c>
-      <c r="F56">
+      <c r="G56">
         <v>65</v>
       </c>
-      <c r="J56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>117</v>
       </c>
@@ -3304,16 +3476,19 @@
         <v>57</v>
       </c>
       <c r="E57">
+        <v>57</v>
+      </c>
+      <c r="F57">
         <v>58</v>
       </c>
-      <c r="F57">
+      <c r="G57">
         <v>64</v>
       </c>
-      <c r="J57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>118</v>
       </c>
@@ -3327,16 +3502,19 @@
         <v>58</v>
       </c>
       <c r="E58">
+        <v>58</v>
+      </c>
+      <c r="F58">
         <v>59</v>
       </c>
-      <c r="F58">
+      <c r="G58">
         <v>63</v>
       </c>
-      <c r="J58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>119</v>
       </c>
@@ -3350,19 +3528,22 @@
         <v>59</v>
       </c>
       <c r="E59">
+        <v>59</v>
+      </c>
+      <c r="F59">
         <v>60</v>
       </c>
-      <c r="F59">
+      <c r="G59">
         <v>61</v>
       </c>
-      <c r="G59">
+      <c r="H59">
         <v>62</v>
       </c>
-      <c r="J59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>120</v>
       </c>
@@ -3375,11 +3556,14 @@
       <c r="D60">
         <v>60</v>
       </c>
-      <c r="J60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E60">
+        <v>60</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>121</v>
       </c>
@@ -3392,11 +3576,14 @@
       <c r="D61">
         <v>61</v>
       </c>
-      <c r="J61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E61">
+        <v>61</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>122</v>
       </c>
@@ -3409,11 +3596,14 @@
       <c r="D62">
         <v>62</v>
       </c>
-      <c r="J62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E62">
+        <v>62</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>123</v>
       </c>
@@ -3426,11 +3616,14 @@
       <c r="D63">
         <v>63</v>
       </c>
-      <c r="J63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E63">
+        <v>63</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>124</v>
       </c>
@@ -3443,11 +3636,14 @@
       <c r="D64">
         <v>64</v>
       </c>
-      <c r="J64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E64">
+        <v>64</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>125</v>
       </c>
@@ -3460,11 +3656,14 @@
       <c r="D65">
         <v>65</v>
       </c>
-      <c r="J65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E65">
+        <v>65</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>126</v>
       </c>
@@ -3477,11 +3676,14 @@
       <c r="D66">
         <v>66</v>
       </c>
-      <c r="J66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E66">
+        <v>66</v>
+      </c>
+      <c r="K66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>127</v>
       </c>
@@ -3495,13 +3697,16 @@
         <v>67</v>
       </c>
       <c r="E67">
+        <v>67</v>
+      </c>
+      <c r="F67">
         <v>68</v>
       </c>
-      <c r="J67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>128</v>
       </c>
@@ -3514,11 +3719,15 @@
       <c r="D68">
         <v>68</v>
       </c>
-      <c r="J68">
+      <c r="E68">
+        <v>68</v>
+      </c>
+      <c r="K68">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K68" xr:uid="{4B166655-9E2D-6541-A5DE-A490A113C8C8}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>